<commit_message>
firstt draft of drag drop BO changes
</commit_message>
<xml_diff>
--- a/invoice_automation/generated_invoices/INV-FY2526-101.xlsx
+++ b/invoice_automation/generated_invoices/INV-FY2526-101.xlsx
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C12" s="23" t="inlineStr">
         <is>
-          <t>Napptix</t>
+          <t>Yazle Marketing Management</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="F12" s="35" t="inlineStr">
         <is>
-          <t>02/02/2026</t>
+          <t>03/02/2026</t>
         </is>
       </c>
       <c r="G12" s="3" t="n"/>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="C13" s="42" t="inlineStr">
         <is>
-          <t>Napptix Address v1</t>
+          <t>Napptix test Address</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="F13" s="35" t="inlineStr">
         <is>
-          <t>04/03/2026</t>
+          <t>05/03/2026</t>
         </is>
       </c>
       <c r="G13" s="3" t="n"/>
@@ -1319,7 +1319,7 @@
       <c r="B14" s="22" t="n"/>
       <c r="C14" s="42" t="inlineStr">
         <is>
-          <t>Napptix Address v1</t>
+          <t>Napptix test Address</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -1340,7 +1340,7 @@
       <c r="B15" s="22" t="n"/>
       <c r="C15" s="42" t="inlineStr">
         <is>
-          <t>Napptix Address v1</t>
+          <t>Napptix test Address</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="F15" s="36" t="inlineStr">
         <is>
-          <t>NAPP|26|02</t>
+          <t>PD25|22041|4</t>
         </is>
       </c>
       <c r="G15" s="3" t="n"/>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="C16" s="24" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>100041433200003</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -1444,17 +1444,17 @@
       </c>
       <c r="C21" s="41" t="inlineStr">
         <is>
-          <t>Napp test delivery</t>
+          <t>Campaign Name</t>
         </is>
       </c>
       <c r="D21" s="39" t="n">
-        <v>100000</v>
+        <v>2025</v>
       </c>
       <c r="E21" s="55" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F21" s="55" t="n">
-        <v>1000</v>
+        <v>28.35</v>
       </c>
       <c r="G21" s="3" t="n"/>
     </row>
@@ -1496,7 +1496,7 @@
         </is>
       </c>
       <c r="F25" s="56" t="n">
-        <v>1000</v>
+        <v>28.35</v>
       </c>
       <c r="G25" s="3" t="n"/>
     </row>
@@ -1509,15 +1509,17 @@
       </c>
       <c r="C26" s="57" t="inlineStr">
         <is>
-          <t>ONE THOUSAND FIFTY DOLLARS</t>
+          <t>TWENTY NINE DOLLARS AND SEVENTY SEVEN CENTS</t>
         </is>
       </c>
       <c r="D26" s="9" t="n"/>
-      <c r="E26" s="46" t="n">
-        <v>5</v>
+      <c r="E26" s="46" t="inlineStr">
+        <is>
+          <t>VAT(5%)</t>
+        </is>
       </c>
       <c r="F26" s="56" t="n">
-        <v>50</v>
+        <v>1.4175</v>
       </c>
       <c r="G26" s="3" t="n"/>
     </row>

</xml_diff>